<commit_message>
Ajout élèves dans fichier billeterie
</commit_message>
<xml_diff>
--- a/template/billeterie.xlsx
+++ b/template/billeterie.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10112"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/etiennerivard/notes_de_cours/support/template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE3861F1-D157-CA40-863B-815B2BFA0953}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F90D0906-EF3D-9041-A409-F2F94665B5B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" xr2:uid="{DF9C8B8D-C7CB-4E48-96BB-D75396ED2350}"/>
+    <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="15560" xr2:uid="{DF9C8B8D-C7CB-4E48-96BB-D75396ED2350}"/>
   </bookViews>
   <sheets>
     <sheet name="liste" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>Équipe</t>
   </si>
@@ -83,20 +83,110 @@
     <t>[https://victo12.on.spiceworks.com](https://victo12.on.spiceworks.com)</t>
   </si>
   <si>
-    <t>&lt;br/&gt;</t>
+    <t>Mathieu Cousança&lt;br/&gt;Albion Selimaj&lt;br/&gt;Louis Hince&lt;br/&gt;</t>
+  </si>
+  <si>
+    <t>Felix Gagne&lt;br/&gt;Didier Mathieu&lt;br/&gt;Mathis Beaulac&lt;br/&gt;</t>
+  </si>
+  <si>
+    <t>Bryan Dubois&lt;br/&gt;Luka St-Hilaire&lt;br/&gt;Leo Nadeau</t>
+  </si>
+  <si>
+    <t>Anne-Sophie Boily&lt;br/&gt;Benjamin Morin Groleau&lt;br/&gt;Louka Ménard&lt;br/&gt;Gabriel Raby</t>
+  </si>
+  <si>
+    <t>Maxime Vallières&lt;br/&gt;Tommy Fontaine&lt;br/&gt;Hugo Lauzière&lt;br/&gt;Christine Lehoux</t>
+  </si>
+  <si>
+    <t>Groupe</t>
+  </si>
+  <si>
+    <t>[https://victo13.on.spiceworks.com](https://victo13.on.spiceworks.com)</t>
+  </si>
+  <si>
+    <t>Mégan Beaulieu&lt;br/&gt;Félix Lemay Bégin&lt;br/&gt;Loic Tremblay&lt;br/&gt;Laurent Côté</t>
+  </si>
+  <si>
+    <t>Nom équipe</t>
+  </si>
+  <si>
+    <t>Table 4</t>
+  </si>
+  <si>
+    <t>FC PITRE</t>
+  </si>
+  <si>
+    <t>Sym</t>
+  </si>
+  <si>
+    <t>FDM</t>
+  </si>
+  <si>
+    <t>Balançoire</t>
+  </si>
+  <si>
+    <t>chill guys</t>
+  </si>
+  <si>
+    <t>Red Tech</t>
+  </si>
+  <si>
+    <t>Maik Ménard&lt;br/&gt;Yamir Romero&lt;br/&gt;Salomon Geurishom</t>
+  </si>
+  <si>
+    <t>Infotech</t>
+  </si>
+  <si>
+    <t>Kungne Wabo Leah&lt;br/&gt;Mickola Turcotte Fortier&lt;br/&gt;Ben Schalom Kamga&lt;br/&gt;</t>
+  </si>
+  <si>
+    <t>Byte Busters</t>
+  </si>
+  <si>
+    <t>Antoine Perreault&lt;br/&gt;Jayke Bédard&lt;br/&gt;Alexis Bergeron&lt;br/&gt;</t>
+  </si>
+  <si>
+    <t>Salut</t>
+  </si>
+  <si>
+    <t>Yoan Bourassa&lt;br/&gt;Zachary Boisvert&lt;br/&gt;Thomas Noël&lt;br/&gt;Nathan Gagnon</t>
+  </si>
+  <si>
+    <t>TMI</t>
+  </si>
+  <si>
+    <t>Timothe Sevigny&lt;br/&gt;Mouad Rabaaoui&lt;br/&gt;Ismail Hentati&lt;br/&gt;</t>
+  </si>
+  <si>
+    <t>Les outsiders</t>
+  </si>
+  <si>
+    <t>Julien Provencher&lt;br/&gt;Jacob Pilotte&lt;br/&gt;Yahya Diop Diop&lt;br/&gt;Katerie Pariseau</t>
+  </si>
+  <si>
+    <t>Bip-Bip</t>
+  </si>
+  <si>
+    <t>Donovan Hamel&lt;br/&gt;William Vincent&lt;br/&gt;Caleb Wilson&lt;br/&gt;Megan Ramsay</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF616161"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -119,9 +209,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -458,159 +552,254 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0D45217-176D-3B43-A394-6BB062C4D536}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="20.1640625" customWidth="1"/>
-    <col min="3" max="3" width="33.83203125" customWidth="1"/>
+    <col min="4" max="4" width="20.1640625" customWidth="1"/>
+    <col min="5" max="5" width="33.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="C2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="68" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C3" t="s">
+      <c r="E3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" ht="68" x14ac:dyDescent="0.2">
       <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
         <v>3</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="C4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5">
         <v>4</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="C5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" ht="85" x14ac:dyDescent="0.2">
       <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6">
         <v>5</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="C6" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="102" x14ac:dyDescent="0.2">
       <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7">
         <v>6</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="C7" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" ht="85" x14ac:dyDescent="0.2">
       <c r="A8">
+        <v>2</v>
+      </c>
+      <c r="B8">
         <v>7</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="C8" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" ht="85" x14ac:dyDescent="0.2">
       <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9">
         <v>8</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" t="s">
+      <c r="C9" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" ht="68" x14ac:dyDescent="0.2">
       <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10">
         <v>9</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" t="s">
+      <c r="C10" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E10" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" ht="85" x14ac:dyDescent="0.2">
       <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11">
         <v>10</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" t="s">
+      <c r="C11" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E11" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" ht="68" x14ac:dyDescent="0.2">
       <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="B12">
         <v>11</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C12" t="s">
+      <c r="C12" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E12" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" ht="85" x14ac:dyDescent="0.2">
       <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="B13">
         <v>12</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C13" t="s">
+      <c r="C13" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E13" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="85" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>1</v>
+      </c>
+      <c r="B14">
+        <v>13</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E14" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changer Leo de groupe
</commit_message>
<xml_diff>
--- a/template/billeterie.xlsx
+++ b/template/billeterie.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10112"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/etiennerivard/notes_de_cours/support/template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F90D0906-EF3D-9041-A409-F2F94665B5B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42319EDF-A789-9B4E-8CB9-B32FEF10966F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="15560" xr2:uid="{DF9C8B8D-C7CB-4E48-96BB-D75396ED2350}"/>
   </bookViews>
@@ -89,9 +89,6 @@
     <t>Felix Gagne&lt;br/&gt;Didier Mathieu&lt;br/&gt;Mathis Beaulac&lt;br/&gt;</t>
   </si>
   <si>
-    <t>Bryan Dubois&lt;br/&gt;Luka St-Hilaire&lt;br/&gt;Leo Nadeau</t>
-  </si>
-  <si>
     <t>Anne-Sophie Boily&lt;br/&gt;Benjamin Morin Groleau&lt;br/&gt;Louka Ménard&lt;br/&gt;Gabriel Raby</t>
   </si>
   <si>
@@ -143,9 +140,6 @@
     <t>Byte Busters</t>
   </si>
   <si>
-    <t>Antoine Perreault&lt;br/&gt;Jayke Bédard&lt;br/&gt;Alexis Bergeron&lt;br/&gt;</t>
-  </si>
-  <si>
     <t>Salut</t>
   </si>
   <si>
@@ -168,6 +162,12 @@
   </si>
   <si>
     <t>Donovan Hamel&lt;br/&gt;William Vincent&lt;br/&gt;Caleb Wilson&lt;br/&gt;Megan Ramsay</t>
+  </si>
+  <si>
+    <t>Bryan Dubois&lt;br/&gt;Luka St-Hilaire</t>
+  </si>
+  <si>
+    <t>Antoine Perreault&lt;br/&gt;Jayke Bédard&lt;br/&gt;Alexis Bergeron&lt;br/&gt;Leo Nadeau</t>
   </si>
 </sst>
 </file>
@@ -554,8 +554,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0D45217-176D-3B43-A394-6BB062C4D536}">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -566,13 +566,13 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
@@ -581,7 +581,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2</v>
       </c>
@@ -589,10 +589,10 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>17</v>
+        <v>42</v>
       </c>
       <c r="E2" t="s">
         <v>3</v>
@@ -606,7 +606,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>15</v>
@@ -623,10 +623,10 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E4" t="s">
         <v>5</v>
@@ -640,7 +640,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>16</v>
@@ -657,10 +657,10 @@
         <v>5</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E6" t="s">
         <v>7</v>
@@ -674,10 +674,10 @@
         <v>6</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E7" t="s">
         <v>8</v>
@@ -691,10 +691,10 @@
         <v>7</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E8" t="s">
         <v>9</v>
@@ -708,16 +708,16 @@
         <v>8</v>
       </c>
       <c r="C9" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>33</v>
       </c>
       <c r="E9" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" ht="85" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1</v>
       </c>
@@ -725,10 +725,10 @@
         <v>9</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="E10" t="s">
         <v>11</v>
@@ -742,10 +742,10 @@
         <v>10</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E11" t="s">
         <v>12</v>
@@ -759,10 +759,10 @@
         <v>11</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E12" t="s">
         <v>13</v>
@@ -776,10 +776,10 @@
         <v>12</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E13" t="s">
         <v>14</v>
@@ -793,13 +793,13 @@
         <v>13</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>